<commit_message>
optimization in the model get distance
</commit_message>
<xml_diff>
--- a/Semantle_AI/profile_results.xlsx
+++ b/Semantle_AI/profile_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/PycharmProjects/SE_Project_Semantle/Semantle_AI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE9BD02-59EA-3E4E-AAF9-BEDC645C039B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4BB2E0-2C4C-464B-AADE-045F1D2C0438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,6 +335,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -679,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -690,7 +691,7 @@
     <col min="1" max="1" width="124" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -965,7 +966,7 @@
         <v>509.28651283400001</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -982,7 +983,7 @@
         <v>1.66E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>1.122666E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1016,7 +1017,7 @@
         <v>1.41958E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>1.2079999999999999E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>2.0474375E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1067,7 +1068,7 @@
         <v>2.9200000000000002E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>509.29278341700001</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>4.8373000000000013E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1118,7 +1119,7 @@
         <v>2.4411670000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>1.0987919999999999E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>1.1211249999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>5.9170000000000003E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1185,8 +1186,9 @@
       <c r="E29">
         <v>9.8931250000000009E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>2.1670000000000002E-6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>2.1670000000000002E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>

</xml_diff>